<commit_message>
Add more Mende gold
</commit_message>
<xml_diff>
--- a/gold_data/Mende_gold.xlsx
+++ b/gold_data/Mende_gold.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9480" windowHeight="14460" tabRatio="500"/>
+    <workbookView xWindow="160" yWindow="0" windowWidth="12020" windowHeight="9900" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1601" uniqueCount="1512">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1932" uniqueCount="1815">
   <si>
     <t>Bafa</t>
   </si>
@@ -4556,6 +4556,915 @@
   </si>
   <si>
     <t>I will help you to learn the work</t>
+  </si>
+  <si>
+    <t>Tisa buwae</t>
+  </si>
+  <si>
+    <t>Good morning teacher</t>
+  </si>
+  <si>
+    <t>Kini buwae bi siɛ gbɔ jia a bie?</t>
+  </si>
+  <si>
+    <t>Good morning sir, how are you what is your mission?</t>
+  </si>
+  <si>
+    <t>Ngi wa nye loi lɔ hinda hungbɛ ma</t>
+  </si>
+  <si>
+    <t>I've come to enquire about my child</t>
+  </si>
+  <si>
+    <t>A gbɛ</t>
+  </si>
+  <si>
+    <t>What for</t>
+  </si>
+  <si>
+    <t>Sia ngi yehelokoi na sukuihun</t>
+  </si>
+  <si>
+    <t>About his progress and behaviour in school</t>
+  </si>
+  <si>
+    <t>Bi loi biyei?</t>
+  </si>
+  <si>
+    <t>What is your child's name?</t>
+  </si>
+  <si>
+    <t>Ngi laa Buakei Same</t>
+  </si>
+  <si>
+    <t>His name is Bockarie Sama</t>
+  </si>
+  <si>
+    <t>Oo! Ngi ngi gɔɔlɔ, I nya klasihunlɔ</t>
+  </si>
+  <si>
+    <t>Ngi nemahun le ngɔ</t>
+  </si>
+  <si>
+    <t>Kɛ a sɛi waa glua klasihun.</t>
+  </si>
+  <si>
+    <t>Nya pen ngɛ gii hungɛ va a bie kɔɔ bi ngi lahin</t>
+  </si>
+  <si>
+    <t>Ah! I know him, he is in my class</t>
+  </si>
+  <si>
+    <t>He is very clever</t>
+  </si>
+  <si>
+    <t>But he is very playful in class</t>
+  </si>
+  <si>
+    <t>Infact I was thinking of telling you so that you will warn him</t>
+  </si>
+  <si>
+    <t>Tisa bi siɛ ka na le ma na, nya logoi bi kpɔma yɛ nya ma ye hindei ngihun, gbɛva ndoi ta numu yila woo ii le. Ya yama lawo ngi ma nahin a we I luwa</t>
+  </si>
+  <si>
+    <t>Thank you very much, teacher, only that I want you to help me with this matter because a child does not belong to one person. Always keep an eye on him so that he can have some fear</t>
+  </si>
+  <si>
+    <t>Pa kulugoi ye ngaa</t>
+  </si>
+  <si>
+    <t>O.k. sir</t>
+  </si>
+  <si>
+    <t>Ngaa mua bie gɔyia le? Nga yaa na a ngi yaabɛ</t>
+  </si>
+  <si>
+    <t>I hope it is a compromise between us. I will now keep watching him</t>
+  </si>
+  <si>
+    <t>Kɛ tamia tisa</t>
+  </si>
+  <si>
+    <t>O.k. see you teacher</t>
+  </si>
+  <si>
+    <t>Ba ya a foo nyama</t>
+  </si>
+  <si>
+    <t>Please be visiting me</t>
+  </si>
+  <si>
+    <t>Alright. See you</t>
+  </si>
+  <si>
+    <t>Gbe a ngendei</t>
+  </si>
+  <si>
+    <t>What is your mission this morning?</t>
+  </si>
+  <si>
+    <t>Gbɛ va</t>
+  </si>
+  <si>
+    <t>Nya loi lɔ kaa madihuma?</t>
+  </si>
+  <si>
+    <t>Is my child serious over his work?</t>
+  </si>
+  <si>
+    <t>A waa suku wati gbi?</t>
+  </si>
+  <si>
+    <t>Does he come to school always?</t>
+  </si>
+  <si>
+    <t>Wua wu dei we ti wa a navo?</t>
+  </si>
+  <si>
+    <t>Did you ask them to bring money?</t>
+  </si>
+  <si>
+    <t>Ngi wa nya loi hunveima</t>
+  </si>
+  <si>
+    <t>I have come to obtain permision for my child</t>
+  </si>
+  <si>
+    <t>Bi loi ju yukpa gɔ wa</t>
+  </si>
+  <si>
+    <t>Your child is very troublesome</t>
+  </si>
+  <si>
+    <t>Bi loi ii baa gɔɔ numugbima</t>
+  </si>
+  <si>
+    <t>Your child has no respect for anyone</t>
+  </si>
+  <si>
+    <t>Bi loi lɔ wa koɛ madihuma</t>
+  </si>
+  <si>
+    <t>Your child is very hard working/studies hard</t>
+  </si>
+  <si>
+    <t>Ya pie I ya humbu a wa sukuihun</t>
+  </si>
+  <si>
+    <t>See that he always comes to school very early</t>
+  </si>
+  <si>
+    <t>Bukui la tebii ma</t>
+  </si>
+  <si>
+    <t>Put the book on the table</t>
+  </si>
+  <si>
+    <t>Buakei lɔ pɛɛ woma</t>
+  </si>
+  <si>
+    <t>Bockarie is behind the house</t>
+  </si>
+  <si>
+    <t>Nda nya gulɔ</t>
+  </si>
+  <si>
+    <t>Put it infront of me</t>
+  </si>
+  <si>
+    <t>Too ngi yakama</t>
+  </si>
+  <si>
+    <t>Place it by his side</t>
+  </si>
+  <si>
+    <t>Glanga</t>
+  </si>
+  <si>
+    <t>Mahun</t>
+  </si>
+  <si>
+    <t>Top/upon</t>
+  </si>
+  <si>
+    <t>Mbu</t>
+  </si>
+  <si>
+    <t>In/into/under</t>
+  </si>
+  <si>
+    <t>Nduahun</t>
+  </si>
+  <si>
+    <t>Between</t>
+  </si>
+  <si>
+    <t>Nga</t>
+  </si>
+  <si>
+    <t>On/at/in/from</t>
+  </si>
+  <si>
+    <t>Kakahun</t>
+  </si>
+  <si>
+    <t>Side</t>
+  </si>
+  <si>
+    <t>Gulɔ</t>
+  </si>
+  <si>
+    <t>Infront</t>
+  </si>
+  <si>
+    <t>Kohun</t>
+  </si>
+  <si>
+    <t>Inside</t>
+  </si>
+  <si>
+    <t>Nda</t>
+  </si>
+  <si>
+    <t>At</t>
+  </si>
+  <si>
+    <t>Wɛ/vaa</t>
+  </si>
+  <si>
+    <t>For</t>
+  </si>
+  <si>
+    <t>Ndia</t>
+  </si>
+  <si>
+    <t>Between/middle/among</t>
+  </si>
+  <si>
+    <t>Hun</t>
+  </si>
+  <si>
+    <t>In/from/to</t>
+  </si>
+  <si>
+    <t>Woma</t>
+  </si>
+  <si>
+    <t>Va</t>
+  </si>
+  <si>
+    <t>Of/for/to in infinitive mood</t>
+  </si>
+  <si>
+    <t>Tia kpaahun</t>
+  </si>
+  <si>
+    <t>They are in the farm</t>
+  </si>
+  <si>
+    <t>Sao gbuaa kpaahun</t>
+  </si>
+  <si>
+    <t>Sao has come from the farm</t>
+  </si>
+  <si>
+    <t>Mu li kpaahun</t>
+  </si>
+  <si>
+    <t>Let us go to the farm</t>
+  </si>
+  <si>
+    <t>Nya nyahei lɔ pɛɛ bu</t>
+  </si>
+  <si>
+    <t>My wife is in the house</t>
+  </si>
+  <si>
+    <t>Baa li la pɛɛ bu</t>
+  </si>
+  <si>
+    <t>Drive him from the house</t>
+  </si>
+  <si>
+    <t>Gɔne lɔ tibii bu</t>
+  </si>
+  <si>
+    <t>The cat is under the table</t>
+  </si>
+  <si>
+    <t>Jo, ndake galu lolɛ mia foihun?</t>
+  </si>
+  <si>
+    <t>Joe, how many months are there in a year?</t>
+  </si>
+  <si>
+    <t>Ngalu puumahun fele mia foihun</t>
+  </si>
+  <si>
+    <t>There are twelve months in a year</t>
+  </si>
+  <si>
+    <t>Ba gulɔ bi ti laagbawa Mɛnde yeihun?</t>
+  </si>
+  <si>
+    <t>Can you name them in Mende?</t>
+  </si>
+  <si>
+    <t>Kɛ ti laa gɛ a ngɛ</t>
+  </si>
+  <si>
+    <t>Then please show them to me</t>
+  </si>
+  <si>
+    <t>Wolo panda hoe</t>
+  </si>
+  <si>
+    <t>Listen carefully</t>
+  </si>
+  <si>
+    <t>Nga wolo ma, kɛ ba nde lɔ maleigɔ</t>
+  </si>
+  <si>
+    <t>I'm listening, but please say it slowly</t>
+  </si>
+  <si>
+    <t>Pɛgbaa</t>
+  </si>
+  <si>
+    <t>January</t>
+  </si>
+  <si>
+    <t>Vui</t>
+  </si>
+  <si>
+    <t>February</t>
+  </si>
+  <si>
+    <t>Nyawɔlii</t>
+  </si>
+  <si>
+    <t>March</t>
+  </si>
+  <si>
+    <t>Buwui</t>
+  </si>
+  <si>
+    <t>April</t>
+  </si>
+  <si>
+    <t>Gooli</t>
+  </si>
+  <si>
+    <t>May</t>
+  </si>
+  <si>
+    <t>Suɛjuɛi</t>
+  </si>
+  <si>
+    <t>June</t>
+  </si>
+  <si>
+    <t>Nanɔi</t>
+  </si>
+  <si>
+    <t>July</t>
+  </si>
+  <si>
+    <t>Dawii</t>
+  </si>
+  <si>
+    <t>August</t>
+  </si>
+  <si>
+    <t>Saai</t>
+  </si>
+  <si>
+    <t>September</t>
+  </si>
+  <si>
+    <t>Galoi</t>
+  </si>
+  <si>
+    <t>October</t>
+  </si>
+  <si>
+    <t>Lugbuyawui</t>
+  </si>
+  <si>
+    <t>November</t>
+  </si>
+  <si>
+    <t>Pondoi</t>
+  </si>
+  <si>
+    <t>December</t>
+  </si>
+  <si>
+    <t>Bi siɛ ka</t>
+  </si>
+  <si>
+    <t>Thank you very much</t>
+  </si>
+  <si>
+    <t>Fo lolɛ mia hoki yilahun?</t>
+  </si>
+  <si>
+    <t>How many days are there in a week?</t>
+  </si>
+  <si>
+    <t>Fo wɔfila mia hoki yilahun</t>
+  </si>
+  <si>
+    <t>There are seven days in a week</t>
+  </si>
+  <si>
+    <t>Taalata</t>
+  </si>
+  <si>
+    <t>Araba</t>
+  </si>
+  <si>
+    <t>Kini Ɔmɔ buaa-e</t>
+  </si>
+  <si>
+    <t>Hello Mr Momoh</t>
+  </si>
+  <si>
+    <t>Mm, ndiamɔ bi siɛ</t>
+  </si>
+  <si>
+    <t>Hello friend</t>
+  </si>
+  <si>
+    <t>I yena, migbe mia bi kpete yehei latoma?</t>
+  </si>
+  <si>
+    <t>How is it: when are you starting the swamp work?</t>
+  </si>
+  <si>
+    <t>It's already time. I'm only waiting for you to give me some advice on the work</t>
+  </si>
+  <si>
+    <t>Wati hintiama. Bia naalee ngi bi mawulo ma kɔ bi nya lo pema</t>
+  </si>
+  <si>
+    <t>Kɛ ba lilɔ naa bi kpetei lue, bi gaayia, ki bi pujaa. Pen ba ya tato ba mbei saanilɔ, nahineve aa yɛ bi kpɔyɔ a bi gbetei wuja la mbei gugɔ a yɛlanaa hin va</t>
+  </si>
+  <si>
+    <t>You can now go ahead and brush your swamp, clear it and dig it. Before starting, you will be ready for transplanting by the time you finish digging your swamp</t>
+  </si>
+  <si>
+    <t>Ba nya ngɔɔ a mba huun wulɔ</t>
+  </si>
+  <si>
+    <t>Will you give me some?</t>
+  </si>
+  <si>
+    <t>Gbei mba huun gbii bi yeya?</t>
+  </si>
+  <si>
+    <t>Why don't you have some?</t>
+  </si>
+  <si>
+    <t>Kɛ wa sina nga bi gbɔɔ a mba huin</t>
+  </si>
+  <si>
+    <t>Then come tomorrow, I'll give you some</t>
+  </si>
+  <si>
+    <t>E-ye, kɛ nya sina wama</t>
+  </si>
+  <si>
+    <t>O.k. then, I'll come tomorrow</t>
+  </si>
+  <si>
+    <t>Kini Ɔmɔ bianaa</t>
+  </si>
+  <si>
+    <t>Afternoof Mr Momoh</t>
+  </si>
+  <si>
+    <t>Sɛmbɛjɔmui bi ye luvei?</t>
+  </si>
+  <si>
+    <t>How is the day bigman?</t>
+  </si>
+  <si>
+    <t>Nya lɔɔ dɛdɛma. Bi ye gɛlia a kpete yegei?</t>
+  </si>
+  <si>
+    <t>I'm managing. How far have you gone with the swamp work?</t>
+  </si>
+  <si>
+    <t>Mbei vaigoi naa, sina yekei mia nga taato a hinla. Kpetei kpɛɛ wuja goi naa</t>
+  </si>
+  <si>
+    <t>The rice has already germinated I'll start transplanting the day after tomorrow. The swamp is already dug</t>
+  </si>
+  <si>
+    <t>Bi nja we leilɔ plɔtisia ti luahun?</t>
+  </si>
+  <si>
+    <t>Did you make drainages in-between the plots?</t>
+  </si>
+  <si>
+    <t>Ɔɔ, sia le gɛ bi hungɛi la a nge</t>
+  </si>
+  <si>
+    <t>Yes, just as you instructed me the last time</t>
+  </si>
+  <si>
+    <t>Kɛ nya sina wama ngi kpeteihun lɔ. Bi ya mbei hinma, ba ti lootoo waa gblagblaga</t>
+  </si>
+  <si>
+    <t>Then I'll be coming tomorrow to see the swamp. When transplanting the rice, do not cluster them together</t>
+  </si>
+  <si>
+    <t>Ɔ bia vui lɔ sina wa ma bi na lɔ?</t>
+  </si>
+  <si>
+    <t>I suppose you'll be coming tomorrow to see there yourself</t>
+  </si>
+  <si>
+    <t>Kɛ ba nya malelɔ</t>
+  </si>
+  <si>
+    <t>Then you will meet me</t>
+  </si>
+  <si>
+    <t>Mua lɔ</t>
+  </si>
+  <si>
+    <t>We shall see</t>
+  </si>
+  <si>
+    <t>Bembei</t>
+  </si>
+  <si>
+    <t>Fishing net</t>
+  </si>
+  <si>
+    <t>Bumbui</t>
+  </si>
+  <si>
+    <t>Fishing Trap</t>
+  </si>
+  <si>
+    <t>Due</t>
+  </si>
+  <si>
+    <t>Brush</t>
+  </si>
+  <si>
+    <t>Due kpe</t>
+  </si>
+  <si>
+    <t>Brushing time</t>
+  </si>
+  <si>
+    <t>Fɛlei</t>
+  </si>
+  <si>
+    <t>Winnowing time</t>
+  </si>
+  <si>
+    <t>Gaaga kpe</t>
+  </si>
+  <si>
+    <t>Time for clearing after burning</t>
+  </si>
+  <si>
+    <t>Hambui</t>
+  </si>
+  <si>
+    <t>An object made of wire hung over fire for drying fish or meat</t>
+  </si>
+  <si>
+    <t>Kali</t>
+  </si>
+  <si>
+    <t>Kondei</t>
+  </si>
+  <si>
+    <t>Mortar</t>
+  </si>
+  <si>
+    <t>Koni</t>
+  </si>
+  <si>
+    <t>Axe</t>
+  </si>
+  <si>
+    <t>Kɔboi</t>
+  </si>
+  <si>
+    <t>Mat (made out of bamboo)</t>
+  </si>
+  <si>
+    <t>Kpakai</t>
+  </si>
+  <si>
+    <t>Three legged wooden chair typical of Mends - used especially on farms</t>
+  </si>
+  <si>
+    <t>Kpasei</t>
+  </si>
+  <si>
+    <t>Circular object used for climbing palm trees</t>
+  </si>
+  <si>
+    <t>Kpangbei</t>
+  </si>
+  <si>
+    <t>Broom</t>
+  </si>
+  <si>
+    <t>Kpawei</t>
+  </si>
+  <si>
+    <t>Forked stick</t>
+  </si>
+  <si>
+    <t>Kpuloi</t>
+  </si>
+  <si>
+    <t>Gourd/keg</t>
+  </si>
+  <si>
+    <t>Kpoe</t>
+  </si>
+  <si>
+    <t>Farm house</t>
+  </si>
+  <si>
+    <t>Lavulei</t>
+  </si>
+  <si>
+    <t>Sling used for scaring birds</t>
+  </si>
+  <si>
+    <t>Mbahui</t>
+  </si>
+  <si>
+    <t>Seed rice</t>
+  </si>
+  <si>
+    <t>Mbowei</t>
+  </si>
+  <si>
+    <t>Knife</t>
+  </si>
+  <si>
+    <t>Mbale bowei</t>
+  </si>
+  <si>
+    <t>Sickle/knife used for cutting rice</t>
+  </si>
+  <si>
+    <t>Ndoi bowei</t>
+  </si>
+  <si>
+    <t>Brushing knife</t>
+  </si>
+  <si>
+    <t>Mbogbei</t>
+  </si>
+  <si>
+    <t>Cutlass</t>
+  </si>
+  <si>
+    <t>Pɔ bogbei</t>
+  </si>
+  <si>
+    <t>Cutlass for cutting down trees</t>
+  </si>
+  <si>
+    <t>Ndɔgboi</t>
+  </si>
+  <si>
+    <t>Bush</t>
+  </si>
+  <si>
+    <t>Ndoli</t>
+  </si>
+  <si>
+    <t>Ngɔmbui</t>
+  </si>
+  <si>
+    <t>Fire</t>
+  </si>
+  <si>
+    <t>Piyei</t>
+  </si>
+  <si>
+    <t>Container for putting fish while fishing</t>
+  </si>
+  <si>
+    <t>Pɔ kpee</t>
+  </si>
+  <si>
+    <t>Time for cutting down large trees/felling time</t>
+  </si>
+  <si>
+    <t>Kpaa mɔ wati</t>
+  </si>
+  <si>
+    <t>Burning time</t>
+  </si>
+  <si>
+    <t>Mbawa kpee</t>
+  </si>
+  <si>
+    <t>Ploughing time</t>
+  </si>
+  <si>
+    <t>Gugbia kpee</t>
+  </si>
+  <si>
+    <t>Weeding time</t>
+  </si>
+  <si>
+    <t>Mbale kpee</t>
+  </si>
+  <si>
+    <t>Harvest season</t>
+  </si>
+  <si>
+    <t>Mɔtu kpee</t>
+  </si>
+  <si>
+    <t>Period of waiting for first rain before ploughing</t>
+  </si>
+  <si>
+    <t>Mba wufoi</t>
+  </si>
+  <si>
+    <t>Newly ploughed land</t>
+  </si>
+  <si>
+    <t>Mba vai</t>
+  </si>
+  <si>
+    <t>Germinated rice</t>
+  </si>
+  <si>
+    <t>Lobai</t>
+  </si>
+  <si>
+    <t>Unploughed land</t>
+  </si>
+  <si>
+    <t>Glangle</t>
+  </si>
+  <si>
+    <t>Gathering and clearing of unburnt shrubs</t>
+  </si>
+  <si>
+    <t>Nyahagaa ti lolɛ bi yeya?</t>
+  </si>
+  <si>
+    <t>How many wives have you</t>
+  </si>
+  <si>
+    <t>Nya nyahin yakpe</t>
+  </si>
+  <si>
+    <t>I have only one wife</t>
+  </si>
+  <si>
+    <t>Nya nyahangaa ti lɔɔlu</t>
+  </si>
+  <si>
+    <t>I have five wives</t>
+  </si>
+  <si>
+    <t>Nya nyahin haa vonu</t>
+  </si>
+  <si>
+    <t>My wife died last year</t>
+  </si>
+  <si>
+    <t>Nya nyahin ii ya ndo lei</t>
+  </si>
+  <si>
+    <t>My wife hasn't a child yet</t>
+  </si>
+  <si>
+    <t>Nya legaa ti nge lɔ</t>
+  </si>
+  <si>
+    <t>This is my chilldren's mother</t>
+  </si>
+  <si>
+    <t>Nyaha ii nya yeya lɛ</t>
+  </si>
+  <si>
+    <t>I don't have a wife yet</t>
+  </si>
+  <si>
+    <t>Kini Blɛma biana</t>
+  </si>
+  <si>
+    <t>Goodday Mr Brima</t>
+  </si>
+  <si>
+    <t>Yes, goodday friend</t>
+  </si>
+  <si>
+    <t>Wa mu mɛhɛn mɛɛ</t>
+  </si>
+  <si>
+    <t>Come and let's eat</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ɛ</t>
+  </si>
+  <si>
+    <t>Ɛnɛn, ndake na gbatɛgoi na</t>
+  </si>
+  <si>
+    <t>O.k. I'm alright now/I'm fed</t>
+  </si>
+  <si>
+    <t>Ndake, wa bɛ hɔ bi kulo mɛ</t>
+  </si>
+  <si>
+    <t>Man, come and have a bit at least</t>
+  </si>
+  <si>
+    <t>Tɔnya mia, kɛ ndake genda mɛhɛn mia ha ngi mia, ye kove mia nya ma. Kɔnɛ le I ye a wati yeka</t>
+  </si>
+  <si>
+    <t>That's true, but man, I have eaten some morning food today and I'm still fed. Please let it be another time</t>
+  </si>
+  <si>
+    <t>Mm, ngi humɛinga ye</t>
+  </si>
+  <si>
+    <t>O.k. I've heard you</t>
+  </si>
+  <si>
+    <t>Kɛ gbɛ ngi fo teihun nya wama</t>
+  </si>
+  <si>
+    <t>Let me go to town, I'll be back</t>
+  </si>
+  <si>
+    <t>E-ye, malɔ</t>
+  </si>
+  <si>
+    <t>Nya govengoi</t>
+  </si>
+  <si>
+    <t>I'm alright/I'm fed</t>
+  </si>
+  <si>
+    <t>Nya foma teihun ngi wa</t>
+  </si>
+  <si>
+    <t>I'm going to town and back</t>
+  </si>
+  <si>
+    <t>Tɔkopɛpɛ</t>
+  </si>
+  <si>
+    <t>Taking food with your hands at a faster rate</t>
+  </si>
+  <si>
+    <t>Kavei</t>
+  </si>
+  <si>
+    <t>Taking too much food at one go</t>
+  </si>
+  <si>
+    <t>Bi liingɔ wa</t>
+  </si>
+  <si>
+    <t>You are gluttinous</t>
+  </si>
+  <si>
+    <t>Bi lamingɔ wa</t>
+  </si>
+  <si>
+    <t>Bi hataigɔ</t>
+  </si>
+  <si>
+    <t>Bi mɛhɛnhindago</t>
+  </si>
+  <si>
+    <t>You are gluttinous (never satisfied with food)</t>
+  </si>
+  <si>
+    <t>Bi nɛhɛngɔ wa</t>
+  </si>
+  <si>
+    <t>You like to stand by for people's food</t>
+  </si>
+  <si>
+    <t>Bi vofulangɔ</t>
+  </si>
+  <si>
+    <t>You are voracious</t>
   </si>
 </sst>
 </file>
@@ -4641,7 +5550,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="74">
+  <cellStyleXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4716,6 +5625,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -4726,7 +5641,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="74">
+  <cellStyles count="80">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -4765,6 +5680,9 @@
     <cellStyle name="Followed Hyperlink" xfId="69" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="71" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="73" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="75" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="77" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="79" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -4800,6 +5718,9 @@
     <cellStyle name="Hyperlink" xfId="68" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="70" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="72" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="74" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="76" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="78" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -5129,10 +6050,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E794"/>
+  <dimension ref="A1:E960"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A763" workbookViewId="0">
-      <selection activeCell="B792" sqref="B792"/>
+    <sheetView tabSelected="1" topLeftCell="A949" workbookViewId="0">
+      <selection activeCell="B963" sqref="B963"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -14303,6 +15224,1826 @@
       </c>
       <c r="C794" t="s">
         <v>1511</v>
+      </c>
+    </row>
+    <row r="795" spans="1:3">
+      <c r="A795">
+        <v>60</v>
+      </c>
+      <c r="B795" t="s">
+        <v>1512</v>
+      </c>
+      <c r="C795" t="s">
+        <v>1513</v>
+      </c>
+    </row>
+    <row r="796" spans="1:3">
+      <c r="A796">
+        <v>60</v>
+      </c>
+      <c r="B796" t="s">
+        <v>1514</v>
+      </c>
+      <c r="C796" t="s">
+        <v>1515</v>
+      </c>
+    </row>
+    <row r="797" spans="1:3">
+      <c r="A797">
+        <v>60</v>
+      </c>
+      <c r="B797" t="s">
+        <v>1516</v>
+      </c>
+      <c r="C797" t="s">
+        <v>1517</v>
+      </c>
+    </row>
+    <row r="798" spans="1:3">
+      <c r="A798">
+        <v>60</v>
+      </c>
+      <c r="B798" t="s">
+        <v>1518</v>
+      </c>
+      <c r="C798" t="s">
+        <v>1519</v>
+      </c>
+    </row>
+    <row r="799" spans="1:3">
+      <c r="A799">
+        <v>60</v>
+      </c>
+      <c r="B799" t="s">
+        <v>1520</v>
+      </c>
+      <c r="C799" t="s">
+        <v>1521</v>
+      </c>
+    </row>
+    <row r="800" spans="1:3">
+      <c r="A800">
+        <v>60</v>
+      </c>
+      <c r="B800" t="s">
+        <v>1522</v>
+      </c>
+      <c r="C800" t="s">
+        <v>1523</v>
+      </c>
+    </row>
+    <row r="801" spans="1:3">
+      <c r="A801">
+        <v>60</v>
+      </c>
+      <c r="B801" t="s">
+        <v>1524</v>
+      </c>
+      <c r="C801" t="s">
+        <v>1525</v>
+      </c>
+    </row>
+    <row r="802" spans="1:3">
+      <c r="A802">
+        <v>60</v>
+      </c>
+      <c r="B802" t="s">
+        <v>1526</v>
+      </c>
+      <c r="C802" t="s">
+        <v>1530</v>
+      </c>
+    </row>
+    <row r="803" spans="1:3">
+      <c r="A803">
+        <v>60</v>
+      </c>
+      <c r="B803" t="s">
+        <v>1527</v>
+      </c>
+      <c r="C803" t="s">
+        <v>1531</v>
+      </c>
+    </row>
+    <row r="804" spans="1:3">
+      <c r="A804">
+        <v>60</v>
+      </c>
+      <c r="B804" t="s">
+        <v>1528</v>
+      </c>
+      <c r="C804" t="s">
+        <v>1532</v>
+      </c>
+    </row>
+    <row r="805" spans="1:3">
+      <c r="A805">
+        <v>60</v>
+      </c>
+      <c r="B805" t="s">
+        <v>1529</v>
+      </c>
+      <c r="C805" t="s">
+        <v>1533</v>
+      </c>
+    </row>
+    <row r="806" spans="1:3">
+      <c r="A806">
+        <v>60</v>
+      </c>
+      <c r="B806" t="s">
+        <v>1534</v>
+      </c>
+      <c r="C806" t="s">
+        <v>1535</v>
+      </c>
+    </row>
+    <row r="807" spans="1:3">
+      <c r="A807">
+        <v>62</v>
+      </c>
+      <c r="B807" t="s">
+        <v>1536</v>
+      </c>
+      <c r="C807" t="s">
+        <v>1537</v>
+      </c>
+    </row>
+    <row r="808" spans="1:3">
+      <c r="A808">
+        <v>62</v>
+      </c>
+      <c r="B808" t="s">
+        <v>1538</v>
+      </c>
+      <c r="C808" t="s">
+        <v>1539</v>
+      </c>
+    </row>
+    <row r="809" spans="1:3">
+      <c r="A809">
+        <v>62</v>
+      </c>
+      <c r="B809" t="s">
+        <v>1540</v>
+      </c>
+      <c r="C809" t="s">
+        <v>1541</v>
+      </c>
+    </row>
+    <row r="810" spans="1:3">
+      <c r="A810">
+        <v>62</v>
+      </c>
+      <c r="B810" t="s">
+        <v>1542</v>
+      </c>
+      <c r="C810" t="s">
+        <v>1543</v>
+      </c>
+    </row>
+    <row r="811" spans="1:3">
+      <c r="A811">
+        <v>62</v>
+      </c>
+      <c r="B811" t="s">
+        <v>645</v>
+      </c>
+      <c r="C811" t="s">
+        <v>1544</v>
+      </c>
+    </row>
+    <row r="812" spans="1:3">
+      <c r="A812">
+        <v>62</v>
+      </c>
+      <c r="B812" t="s">
+        <v>1545</v>
+      </c>
+      <c r="C812" t="s">
+        <v>1546</v>
+      </c>
+    </row>
+    <row r="813" spans="1:3">
+      <c r="A813">
+        <v>62</v>
+      </c>
+      <c r="B813" t="s">
+        <v>1547</v>
+      </c>
+      <c r="C813" t="s">
+        <v>1519</v>
+      </c>
+    </row>
+    <row r="814" spans="1:3">
+      <c r="A814">
+        <v>62</v>
+      </c>
+      <c r="B814" t="s">
+        <v>1548</v>
+      </c>
+      <c r="C814" t="s">
+        <v>1549</v>
+      </c>
+    </row>
+    <row r="815" spans="1:3">
+      <c r="A815">
+        <v>62</v>
+      </c>
+      <c r="B815" t="s">
+        <v>1550</v>
+      </c>
+      <c r="C815" t="s">
+        <v>1551</v>
+      </c>
+    </row>
+    <row r="816" spans="1:3">
+      <c r="A816">
+        <v>62</v>
+      </c>
+      <c r="B816" t="s">
+        <v>1552</v>
+      </c>
+      <c r="C816" t="s">
+        <v>1553</v>
+      </c>
+    </row>
+    <row r="817" spans="1:3">
+      <c r="A817">
+        <v>62</v>
+      </c>
+      <c r="B817" t="s">
+        <v>1554</v>
+      </c>
+      <c r="C817" t="s">
+        <v>1555</v>
+      </c>
+    </row>
+    <row r="818" spans="1:3">
+      <c r="A818">
+        <v>62</v>
+      </c>
+      <c r="B818" t="s">
+        <v>1556</v>
+      </c>
+      <c r="C818" t="s">
+        <v>1557</v>
+      </c>
+    </row>
+    <row r="819" spans="1:3">
+      <c r="A819">
+        <v>62</v>
+      </c>
+      <c r="B819" t="s">
+        <v>1558</v>
+      </c>
+      <c r="C819" t="s">
+        <v>1559</v>
+      </c>
+    </row>
+    <row r="820" spans="1:3">
+      <c r="A820">
+        <v>62</v>
+      </c>
+      <c r="B820" t="s">
+        <v>1560</v>
+      </c>
+      <c r="C820" t="s">
+        <v>1561</v>
+      </c>
+    </row>
+    <row r="821" spans="1:3">
+      <c r="A821">
+        <v>62</v>
+      </c>
+      <c r="B821" t="s">
+        <v>1562</v>
+      </c>
+      <c r="C821" t="s">
+        <v>1563</v>
+      </c>
+    </row>
+    <row r="822" spans="1:3">
+      <c r="A822">
+        <v>62</v>
+      </c>
+      <c r="B822" t="s">
+        <v>1564</v>
+      </c>
+      <c r="C822" t="s">
+        <v>1565</v>
+      </c>
+    </row>
+    <row r="823" spans="1:3">
+      <c r="A823">
+        <v>62</v>
+      </c>
+      <c r="B823" t="s">
+        <v>1566</v>
+      </c>
+      <c r="C823" t="s">
+        <v>1567</v>
+      </c>
+    </row>
+    <row r="824" spans="1:3">
+      <c r="A824">
+        <v>62</v>
+      </c>
+      <c r="B824" t="s">
+        <v>1568</v>
+      </c>
+      <c r="C824" t="s">
+        <v>1569</v>
+      </c>
+    </row>
+    <row r="825" spans="1:3">
+      <c r="A825">
+        <v>62</v>
+      </c>
+      <c r="B825" t="s">
+        <v>1570</v>
+      </c>
+      <c r="C825" t="s">
+        <v>1571</v>
+      </c>
+    </row>
+    <row r="826" spans="1:3">
+      <c r="A826">
+        <v>63</v>
+      </c>
+      <c r="B826" t="s">
+        <v>1572</v>
+      </c>
+      <c r="C826" t="s">
+        <v>1132</v>
+      </c>
+    </row>
+    <row r="827" spans="1:3">
+      <c r="A827">
+        <v>63</v>
+      </c>
+      <c r="B827" t="s">
+        <v>1573</v>
+      </c>
+      <c r="C827" t="s">
+        <v>1574</v>
+      </c>
+    </row>
+    <row r="828" spans="1:3">
+      <c r="A828">
+        <v>63</v>
+      </c>
+      <c r="B828" t="s">
+        <v>1575</v>
+      </c>
+      <c r="C828" t="s">
+        <v>1576</v>
+      </c>
+    </row>
+    <row r="829" spans="1:3">
+      <c r="A829">
+        <v>63</v>
+      </c>
+      <c r="B829" t="s">
+        <v>1577</v>
+      </c>
+      <c r="C829" t="s">
+        <v>1578</v>
+      </c>
+    </row>
+    <row r="830" spans="1:3">
+      <c r="A830">
+        <v>63</v>
+      </c>
+      <c r="B830" t="s">
+        <v>1579</v>
+      </c>
+      <c r="C830" t="s">
+        <v>1580</v>
+      </c>
+    </row>
+    <row r="831" spans="1:3">
+      <c r="A831">
+        <v>63</v>
+      </c>
+      <c r="B831" t="s">
+        <v>1581</v>
+      </c>
+      <c r="C831" t="s">
+        <v>1582</v>
+      </c>
+    </row>
+    <row r="832" spans="1:3">
+      <c r="A832">
+        <v>63</v>
+      </c>
+      <c r="B832" t="s">
+        <v>1583</v>
+      </c>
+      <c r="C832" t="s">
+        <v>1584</v>
+      </c>
+    </row>
+    <row r="833" spans="1:3">
+      <c r="A833">
+        <v>63</v>
+      </c>
+      <c r="B833" t="s">
+        <v>1585</v>
+      </c>
+      <c r="C833" t="s">
+        <v>1586</v>
+      </c>
+    </row>
+    <row r="834" spans="1:3">
+      <c r="A834">
+        <v>63</v>
+      </c>
+      <c r="B834" t="s">
+        <v>1587</v>
+      </c>
+      <c r="C834" t="s">
+        <v>1588</v>
+      </c>
+    </row>
+    <row r="835" spans="1:3">
+      <c r="A835">
+        <v>63</v>
+      </c>
+      <c r="B835" t="s">
+        <v>1589</v>
+      </c>
+      <c r="C835" t="s">
+        <v>1590</v>
+      </c>
+    </row>
+    <row r="836" spans="1:3">
+      <c r="A836">
+        <v>63</v>
+      </c>
+      <c r="B836" t="s">
+        <v>1591</v>
+      </c>
+      <c r="C836" t="s">
+        <v>1592</v>
+      </c>
+    </row>
+    <row r="837" spans="1:3">
+      <c r="A837">
+        <v>63</v>
+      </c>
+      <c r="B837" t="s">
+        <v>1593</v>
+      </c>
+      <c r="C837" t="s">
+        <v>1594</v>
+      </c>
+    </row>
+    <row r="838" spans="1:3">
+      <c r="A838">
+        <v>63</v>
+      </c>
+      <c r="B838" t="s">
+        <v>1595</v>
+      </c>
+      <c r="C838" t="s">
+        <v>1138</v>
+      </c>
+    </row>
+    <row r="839" spans="1:3">
+      <c r="A839">
+        <v>63</v>
+      </c>
+      <c r="B839" t="s">
+        <v>1596</v>
+      </c>
+      <c r="C839" t="s">
+        <v>1597</v>
+      </c>
+    </row>
+    <row r="840" spans="1:3">
+      <c r="A840">
+        <v>63</v>
+      </c>
+      <c r="B840" t="s">
+        <v>1598</v>
+      </c>
+      <c r="C840" t="s">
+        <v>1599</v>
+      </c>
+    </row>
+    <row r="841" spans="1:3">
+      <c r="A841">
+        <v>63</v>
+      </c>
+      <c r="B841" t="s">
+        <v>1600</v>
+      </c>
+      <c r="C841" t="s">
+        <v>1601</v>
+      </c>
+    </row>
+    <row r="842" spans="1:3">
+      <c r="A842">
+        <v>63</v>
+      </c>
+      <c r="B842" t="s">
+        <v>1602</v>
+      </c>
+      <c r="C842" t="s">
+        <v>1603</v>
+      </c>
+    </row>
+    <row r="843" spans="1:3">
+      <c r="A843">
+        <v>63</v>
+      </c>
+      <c r="B843" t="s">
+        <v>1604</v>
+      </c>
+      <c r="C843" t="s">
+        <v>1605</v>
+      </c>
+    </row>
+    <row r="844" spans="1:3">
+      <c r="A844">
+        <v>63</v>
+      </c>
+      <c r="B844" t="s">
+        <v>1606</v>
+      </c>
+      <c r="C844" t="s">
+        <v>1607</v>
+      </c>
+    </row>
+    <row r="845" spans="1:3">
+      <c r="A845">
+        <v>63</v>
+      </c>
+      <c r="B845" t="s">
+        <v>1608</v>
+      </c>
+      <c r="C845" t="s">
+        <v>1609</v>
+      </c>
+    </row>
+    <row r="846" spans="1:3">
+      <c r="A846">
+        <v>65</v>
+      </c>
+      <c r="B846" t="s">
+        <v>1610</v>
+      </c>
+      <c r="C846" t="s">
+        <v>1611</v>
+      </c>
+    </row>
+    <row r="847" spans="1:3">
+      <c r="A847">
+        <v>65</v>
+      </c>
+      <c r="B847" t="s">
+        <v>1612</v>
+      </c>
+      <c r="C847" t="s">
+        <v>1613</v>
+      </c>
+    </row>
+    <row r="848" spans="1:3">
+      <c r="A848">
+        <v>65</v>
+      </c>
+      <c r="B848" t="s">
+        <v>1614</v>
+      </c>
+      <c r="C848" t="s">
+        <v>1615</v>
+      </c>
+    </row>
+    <row r="849" spans="1:3">
+      <c r="A849">
+        <v>65</v>
+      </c>
+      <c r="B849" t="s">
+        <v>1011</v>
+      </c>
+      <c r="C849" t="s">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="850" spans="1:3">
+      <c r="A850">
+        <v>65</v>
+      </c>
+      <c r="B850" t="s">
+        <v>1616</v>
+      </c>
+      <c r="C850" t="s">
+        <v>1617</v>
+      </c>
+    </row>
+    <row r="851" spans="1:3">
+      <c r="A851">
+        <v>65</v>
+      </c>
+      <c r="B851" t="s">
+        <v>1618</v>
+      </c>
+      <c r="C851" t="s">
+        <v>1619</v>
+      </c>
+    </row>
+    <row r="852" spans="1:3">
+      <c r="A852">
+        <v>65</v>
+      </c>
+      <c r="B852" t="s">
+        <v>1620</v>
+      </c>
+      <c r="C852" t="s">
+        <v>1621</v>
+      </c>
+    </row>
+    <row r="853" spans="1:3">
+      <c r="A853">
+        <v>65</v>
+      </c>
+      <c r="B853" t="s">
+        <v>1622</v>
+      </c>
+      <c r="C853" t="s">
+        <v>1623</v>
+      </c>
+    </row>
+    <row r="854" spans="1:3">
+      <c r="A854">
+        <v>65</v>
+      </c>
+      <c r="B854" t="s">
+        <v>1624</v>
+      </c>
+      <c r="C854" t="s">
+        <v>1625</v>
+      </c>
+    </row>
+    <row r="855" spans="1:3">
+      <c r="A855">
+        <v>65</v>
+      </c>
+      <c r="B855" t="s">
+        <v>1626</v>
+      </c>
+      <c r="C855" t="s">
+        <v>1627</v>
+      </c>
+    </row>
+    <row r="856" spans="1:3">
+      <c r="A856">
+        <v>65</v>
+      </c>
+      <c r="B856" t="s">
+        <v>1628</v>
+      </c>
+      <c r="C856" t="s">
+        <v>1629</v>
+      </c>
+    </row>
+    <row r="857" spans="1:3">
+      <c r="A857">
+        <v>65</v>
+      </c>
+      <c r="B857" t="s">
+        <v>1630</v>
+      </c>
+      <c r="C857" t="s">
+        <v>1631</v>
+      </c>
+    </row>
+    <row r="858" spans="1:3">
+      <c r="A858">
+        <v>65</v>
+      </c>
+      <c r="B858" t="s">
+        <v>1632</v>
+      </c>
+      <c r="C858" t="s">
+        <v>1633</v>
+      </c>
+    </row>
+    <row r="859" spans="1:3">
+      <c r="A859">
+        <v>65</v>
+      </c>
+      <c r="B859" t="s">
+        <v>1634</v>
+      </c>
+      <c r="C859" t="s">
+        <v>1635</v>
+      </c>
+    </row>
+    <row r="860" spans="1:3">
+      <c r="A860">
+        <v>65</v>
+      </c>
+      <c r="B860" t="s">
+        <v>1636</v>
+      </c>
+      <c r="C860" t="s">
+        <v>1637</v>
+      </c>
+    </row>
+    <row r="861" spans="1:3">
+      <c r="A861">
+        <v>65</v>
+      </c>
+      <c r="B861" t="s">
+        <v>1638</v>
+      </c>
+      <c r="C861" t="s">
+        <v>1639</v>
+      </c>
+    </row>
+    <row r="862" spans="1:3">
+      <c r="A862">
+        <v>65</v>
+      </c>
+      <c r="B862" t="s">
+        <v>1640</v>
+      </c>
+      <c r="C862" t="s">
+        <v>1641</v>
+      </c>
+    </row>
+    <row r="863" spans="1:3">
+      <c r="A863">
+        <v>65</v>
+      </c>
+      <c r="B863" t="s">
+        <v>1642</v>
+      </c>
+      <c r="C863" t="s">
+        <v>1643</v>
+      </c>
+    </row>
+    <row r="864" spans="1:3">
+      <c r="A864">
+        <v>65</v>
+      </c>
+      <c r="B864" t="s">
+        <v>1644</v>
+      </c>
+      <c r="C864" t="s">
+        <v>1645</v>
+      </c>
+    </row>
+    <row r="865" spans="1:3">
+      <c r="A865">
+        <v>65</v>
+      </c>
+      <c r="B865" t="s">
+        <v>1646</v>
+      </c>
+      <c r="C865" t="s">
+        <v>1647</v>
+      </c>
+    </row>
+    <row r="866" spans="1:3">
+      <c r="A866">
+        <v>65</v>
+      </c>
+      <c r="B866" t="s">
+        <v>1648</v>
+      </c>
+      <c r="C866" t="s">
+        <v>1649</v>
+      </c>
+    </row>
+    <row r="867" spans="1:3">
+      <c r="A867">
+        <v>65</v>
+      </c>
+      <c r="B867" t="s">
+        <v>1650</v>
+      </c>
+      <c r="C867" t="s">
+        <v>1651</v>
+      </c>
+    </row>
+    <row r="868" spans="1:3">
+      <c r="A868">
+        <v>65</v>
+      </c>
+      <c r="B868" t="s">
+        <v>1266</v>
+      </c>
+      <c r="C868" t="s">
+        <v>1267</v>
+      </c>
+    </row>
+    <row r="869" spans="1:3">
+      <c r="A869">
+        <v>65</v>
+      </c>
+      <c r="B869" t="s">
+        <v>1652</v>
+      </c>
+      <c r="C869" t="s">
+        <v>1269</v>
+      </c>
+    </row>
+    <row r="870" spans="1:3">
+      <c r="A870">
+        <v>65</v>
+      </c>
+      <c r="B870" t="s">
+        <v>1653</v>
+      </c>
+      <c r="C870" t="s">
+        <v>1271</v>
+      </c>
+    </row>
+    <row r="871" spans="1:3">
+      <c r="A871">
+        <v>65</v>
+      </c>
+      <c r="B871" t="s">
+        <v>1272</v>
+      </c>
+      <c r="C871" t="s">
+        <v>1273</v>
+      </c>
+    </row>
+    <row r="872" spans="1:3">
+      <c r="A872">
+        <v>65</v>
+      </c>
+      <c r="B872" t="s">
+        <v>1274</v>
+      </c>
+      <c r="C872" t="s">
+        <v>1275</v>
+      </c>
+    </row>
+    <row r="873" spans="1:3">
+      <c r="A873">
+        <v>65</v>
+      </c>
+      <c r="B873" t="s">
+        <v>1279</v>
+      </c>
+      <c r="C873" t="s">
+        <v>1278</v>
+      </c>
+    </row>
+    <row r="874" spans="1:3">
+      <c r="A874">
+        <v>65</v>
+      </c>
+      <c r="B874" t="s">
+        <v>1276</v>
+      </c>
+      <c r="C874" t="s">
+        <v>1277</v>
+      </c>
+    </row>
+    <row r="875" spans="1:3">
+      <c r="A875">
+        <v>66</v>
+      </c>
+      <c r="B875" t="s">
+        <v>1654</v>
+      </c>
+      <c r="C875" t="s">
+        <v>1655</v>
+      </c>
+    </row>
+    <row r="876" spans="1:3">
+      <c r="A876">
+        <v>66</v>
+      </c>
+      <c r="B876" t="s">
+        <v>1656</v>
+      </c>
+      <c r="C876" t="s">
+        <v>1657</v>
+      </c>
+    </row>
+    <row r="877" spans="1:3">
+      <c r="A877">
+        <v>66</v>
+      </c>
+      <c r="B877" t="s">
+        <v>1658</v>
+      </c>
+      <c r="C877" t="s">
+        <v>1659</v>
+      </c>
+    </row>
+    <row r="878" spans="1:3">
+      <c r="A878">
+        <v>66</v>
+      </c>
+      <c r="B878" t="s">
+        <v>1661</v>
+      </c>
+      <c r="C878" t="s">
+        <v>1660</v>
+      </c>
+    </row>
+    <row r="879" spans="1:3">
+      <c r="A879">
+        <v>66</v>
+      </c>
+      <c r="B879" t="s">
+        <v>1662</v>
+      </c>
+      <c r="C879" t="s">
+        <v>1663</v>
+      </c>
+    </row>
+    <row r="880" spans="1:3">
+      <c r="A880">
+        <v>66</v>
+      </c>
+      <c r="B880" t="s">
+        <v>1664</v>
+      </c>
+      <c r="C880" t="s">
+        <v>1665</v>
+      </c>
+    </row>
+    <row r="881" spans="1:3">
+      <c r="A881">
+        <v>66</v>
+      </c>
+      <c r="B881" t="s">
+        <v>1666</v>
+      </c>
+      <c r="C881" t="s">
+        <v>1667</v>
+      </c>
+    </row>
+    <row r="882" spans="1:3">
+      <c r="A882">
+        <v>66</v>
+      </c>
+      <c r="B882" t="s">
+        <v>1011</v>
+      </c>
+      <c r="C882" t="s">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="883" spans="1:3">
+      <c r="A883">
+        <v>66</v>
+      </c>
+      <c r="B883" t="s">
+        <v>1668</v>
+      </c>
+      <c r="C883" t="s">
+        <v>1669</v>
+      </c>
+    </row>
+    <row r="884" spans="1:3">
+      <c r="A884">
+        <v>66</v>
+      </c>
+      <c r="B884" t="s">
+        <v>1670</v>
+      </c>
+      <c r="C884" t="s">
+        <v>1671</v>
+      </c>
+    </row>
+    <row r="885" spans="1:3">
+      <c r="A885">
+        <v>66</v>
+      </c>
+      <c r="B885" t="s">
+        <v>1672</v>
+      </c>
+      <c r="C885" t="s">
+        <v>1673</v>
+      </c>
+    </row>
+    <row r="886" spans="1:3">
+      <c r="A886">
+        <v>66</v>
+      </c>
+      <c r="B886" t="s">
+        <v>1674</v>
+      </c>
+      <c r="C886" t="s">
+        <v>1675</v>
+      </c>
+    </row>
+    <row r="887" spans="1:3">
+      <c r="A887">
+        <v>66</v>
+      </c>
+      <c r="B887" t="s">
+        <v>1676</v>
+      </c>
+      <c r="C887" t="s">
+        <v>1677</v>
+      </c>
+    </row>
+    <row r="888" spans="1:3">
+      <c r="A888">
+        <v>66</v>
+      </c>
+      <c r="B888" t="s">
+        <v>1678</v>
+      </c>
+      <c r="C888" t="s">
+        <v>1679</v>
+      </c>
+    </row>
+    <row r="889" spans="1:3">
+      <c r="A889">
+        <v>67</v>
+      </c>
+      <c r="B889" t="s">
+        <v>1680</v>
+      </c>
+      <c r="C889" t="s">
+        <v>1681</v>
+      </c>
+    </row>
+    <row r="890" spans="1:3">
+      <c r="A890">
+        <v>67</v>
+      </c>
+      <c r="B890" t="s">
+        <v>1682</v>
+      </c>
+      <c r="C890" t="s">
+        <v>1683</v>
+      </c>
+    </row>
+    <row r="891" spans="1:3">
+      <c r="A891">
+        <v>67</v>
+      </c>
+      <c r="B891" t="s">
+        <v>1684</v>
+      </c>
+      <c r="C891" t="s">
+        <v>1685</v>
+      </c>
+    </row>
+    <row r="892" spans="1:3">
+      <c r="A892">
+        <v>67</v>
+      </c>
+      <c r="B892" t="s">
+        <v>1686</v>
+      </c>
+      <c r="C892" t="s">
+        <v>1687</v>
+      </c>
+    </row>
+    <row r="893" spans="1:3">
+      <c r="A893">
+        <v>67</v>
+      </c>
+      <c r="B893" t="s">
+        <v>1011</v>
+      </c>
+      <c r="C893" t="s">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="894" spans="1:3">
+      <c r="A894">
+        <v>67</v>
+      </c>
+      <c r="B894" t="s">
+        <v>1688</v>
+      </c>
+      <c r="C894" t="s">
+        <v>1689</v>
+      </c>
+    </row>
+    <row r="895" spans="1:3">
+      <c r="A895">
+        <v>67</v>
+      </c>
+      <c r="B895" t="s">
+        <v>1690</v>
+      </c>
+      <c r="C895" t="s">
+        <v>1691</v>
+      </c>
+    </row>
+    <row r="896" spans="1:3">
+      <c r="A896">
+        <v>67</v>
+      </c>
+      <c r="B896" t="s">
+        <v>1692</v>
+      </c>
+      <c r="C896" t="s">
+        <v>1693</v>
+      </c>
+    </row>
+    <row r="897" spans="1:3">
+      <c r="A897">
+        <v>67</v>
+      </c>
+      <c r="B897" t="s">
+        <v>1694</v>
+      </c>
+      <c r="C897" t="s">
+        <v>1695</v>
+      </c>
+    </row>
+    <row r="898" spans="1:3">
+      <c r="A898">
+        <v>67</v>
+      </c>
+      <c r="B898" t="s">
+        <v>1696</v>
+      </c>
+      <c r="C898" t="s">
+        <v>1697</v>
+      </c>
+    </row>
+    <row r="899" spans="1:3">
+      <c r="A899">
+        <v>67</v>
+      </c>
+      <c r="B899" t="s">
+        <v>1698</v>
+      </c>
+      <c r="C899" t="s">
+        <v>1699</v>
+      </c>
+    </row>
+    <row r="900" spans="1:3">
+      <c r="A900">
+        <v>67</v>
+      </c>
+      <c r="B900" t="s">
+        <v>1700</v>
+      </c>
+      <c r="C900" t="s">
+        <v>1701</v>
+      </c>
+    </row>
+    <row r="901" spans="1:3">
+      <c r="A901">
+        <v>67</v>
+      </c>
+      <c r="B901" t="s">
+        <v>1702</v>
+      </c>
+      <c r="C901" t="s">
+        <v>1703</v>
+      </c>
+    </row>
+    <row r="902" spans="1:3">
+      <c r="A902">
+        <v>67</v>
+      </c>
+      <c r="B902" t="s">
+        <v>1704</v>
+      </c>
+      <c r="C902" t="s">
+        <v>1705</v>
+      </c>
+    </row>
+    <row r="903" spans="1:3">
+      <c r="A903">
+        <v>67</v>
+      </c>
+      <c r="B903" t="s">
+        <v>1706</v>
+      </c>
+      <c r="C903" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="904" spans="1:3">
+      <c r="A904">
+        <v>67</v>
+      </c>
+      <c r="B904" t="s">
+        <v>1707</v>
+      </c>
+      <c r="C904" t="s">
+        <v>1708</v>
+      </c>
+    </row>
+    <row r="905" spans="1:3">
+      <c r="A905">
+        <v>67</v>
+      </c>
+      <c r="B905" t="s">
+        <v>1709</v>
+      </c>
+      <c r="C905" t="s">
+        <v>1710</v>
+      </c>
+    </row>
+    <row r="906" spans="1:3">
+      <c r="A906">
+        <v>67</v>
+      </c>
+      <c r="B906" t="s">
+        <v>1711</v>
+      </c>
+      <c r="C906" t="s">
+        <v>1712</v>
+      </c>
+    </row>
+    <row r="907" spans="1:3">
+      <c r="A907">
+        <v>67</v>
+      </c>
+      <c r="B907" t="s">
+        <v>1713</v>
+      </c>
+      <c r="C907" t="s">
+        <v>1714</v>
+      </c>
+    </row>
+    <row r="908" spans="1:3">
+      <c r="A908">
+        <v>67</v>
+      </c>
+      <c r="B908" t="s">
+        <v>1715</v>
+      </c>
+      <c r="C908" t="s">
+        <v>1716</v>
+      </c>
+    </row>
+    <row r="909" spans="1:3">
+      <c r="A909">
+        <v>67</v>
+      </c>
+      <c r="B909" t="s">
+        <v>1717</v>
+      </c>
+      <c r="C909" t="s">
+        <v>1718</v>
+      </c>
+    </row>
+    <row r="910" spans="1:3">
+      <c r="A910">
+        <v>67</v>
+      </c>
+      <c r="B910" t="s">
+        <v>1719</v>
+      </c>
+      <c r="C910" t="s">
+        <v>1720</v>
+      </c>
+    </row>
+    <row r="911" spans="1:3">
+      <c r="A911">
+        <v>67</v>
+      </c>
+      <c r="B911" t="s">
+        <v>1721</v>
+      </c>
+      <c r="C911" t="s">
+        <v>1722</v>
+      </c>
+    </row>
+    <row r="912" spans="1:3">
+      <c r="A912">
+        <v>67</v>
+      </c>
+      <c r="B912" t="s">
+        <v>1723</v>
+      </c>
+      <c r="C912" t="s">
+        <v>1724</v>
+      </c>
+    </row>
+    <row r="913" spans="1:3">
+      <c r="A913">
+        <v>67</v>
+      </c>
+      <c r="B913" t="s">
+        <v>1725</v>
+      </c>
+      <c r="C913" t="s">
+        <v>1726</v>
+      </c>
+    </row>
+    <row r="914" spans="1:3">
+      <c r="A914">
+        <v>67</v>
+      </c>
+      <c r="B914" t="s">
+        <v>1727</v>
+      </c>
+      <c r="C914" t="s">
+        <v>1728</v>
+      </c>
+    </row>
+    <row r="915" spans="1:3">
+      <c r="A915">
+        <v>67</v>
+      </c>
+      <c r="B915" t="s">
+        <v>1729</v>
+      </c>
+      <c r="C915" t="s">
+        <v>1730</v>
+      </c>
+    </row>
+    <row r="916" spans="1:3">
+      <c r="A916">
+        <v>67</v>
+      </c>
+      <c r="B916" t="s">
+        <v>1731</v>
+      </c>
+      <c r="C916" t="s">
+        <v>1732</v>
+      </c>
+    </row>
+    <row r="917" spans="1:3">
+      <c r="A917">
+        <v>67</v>
+      </c>
+      <c r="B917" t="s">
+        <v>1733</v>
+      </c>
+      <c r="C917" t="s">
+        <v>1734</v>
+      </c>
+    </row>
+    <row r="918" spans="1:3">
+      <c r="A918">
+        <v>67</v>
+      </c>
+      <c r="B918" t="s">
+        <v>1735</v>
+      </c>
+      <c r="C918" t="s">
+        <v>1736</v>
+      </c>
+    </row>
+    <row r="919" spans="1:3">
+      <c r="A919">
+        <v>67</v>
+      </c>
+      <c r="B919" t="s">
+        <v>1737</v>
+      </c>
+      <c r="C919" t="s">
+        <v>1738</v>
+      </c>
+    </row>
+    <row r="920" spans="1:3">
+      <c r="A920">
+        <v>67</v>
+      </c>
+      <c r="B920" t="s">
+        <v>1739</v>
+      </c>
+      <c r="C920" t="s">
+        <v>1740</v>
+      </c>
+    </row>
+    <row r="921" spans="1:3">
+      <c r="A921">
+        <v>67</v>
+      </c>
+      <c r="B921" t="s">
+        <v>1741</v>
+      </c>
+      <c r="C921" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="922" spans="1:3">
+      <c r="A922">
+        <v>67</v>
+      </c>
+      <c r="B922" t="s">
+        <v>1742</v>
+      </c>
+      <c r="C922" t="s">
+        <v>1743</v>
+      </c>
+    </row>
+    <row r="923" spans="1:3">
+      <c r="A923">
+        <v>67</v>
+      </c>
+      <c r="B923" t="s">
+        <v>1744</v>
+      </c>
+      <c r="C923" t="s">
+        <v>1745</v>
+      </c>
+    </row>
+    <row r="924" spans="1:3">
+      <c r="A924">
+        <v>68</v>
+      </c>
+      <c r="B924" t="s">
+        <v>1746</v>
+      </c>
+      <c r="C924" t="s">
+        <v>1747</v>
+      </c>
+    </row>
+    <row r="925" spans="1:3">
+      <c r="A925">
+        <v>68</v>
+      </c>
+      <c r="B925" t="s">
+        <v>1748</v>
+      </c>
+      <c r="C925" t="s">
+        <v>1749</v>
+      </c>
+    </row>
+    <row r="926" spans="1:3">
+      <c r="A926">
+        <v>68</v>
+      </c>
+      <c r="B926" t="s">
+        <v>1750</v>
+      </c>
+      <c r="C926" t="s">
+        <v>1751</v>
+      </c>
+    </row>
+    <row r="927" spans="1:3">
+      <c r="A927">
+        <v>68</v>
+      </c>
+      <c r="B927" t="s">
+        <v>1752</v>
+      </c>
+      <c r="C927" t="s">
+        <v>1753</v>
+      </c>
+    </row>
+    <row r="928" spans="1:3">
+      <c r="A928">
+        <v>68</v>
+      </c>
+      <c r="B928" t="s">
+        <v>1754</v>
+      </c>
+      <c r="C928" t="s">
+        <v>1755</v>
+      </c>
+    </row>
+    <row r="929" spans="1:3">
+      <c r="A929">
+        <v>68</v>
+      </c>
+      <c r="B929" t="s">
+        <v>1756</v>
+      </c>
+      <c r="C929" t="s">
+        <v>1757</v>
+      </c>
+    </row>
+    <row r="930" spans="1:3">
+      <c r="A930">
+        <v>68</v>
+      </c>
+      <c r="B930" t="s">
+        <v>1758</v>
+      </c>
+      <c r="C930" t="s">
+        <v>1759</v>
+      </c>
+    </row>
+    <row r="931" spans="1:3">
+      <c r="A931">
+        <v>68</v>
+      </c>
+      <c r="B931" t="s">
+        <v>1760</v>
+      </c>
+      <c r="C931" t="s">
+        <v>1761</v>
+      </c>
+    </row>
+    <row r="932" spans="1:3">
+      <c r="A932">
+        <v>68</v>
+      </c>
+      <c r="B932" t="s">
+        <v>1762</v>
+      </c>
+      <c r="C932" t="s">
+        <v>1763</v>
+      </c>
+    </row>
+    <row r="933" spans="1:3">
+      <c r="A933">
+        <v>68</v>
+      </c>
+      <c r="B933" t="s">
+        <v>1764</v>
+      </c>
+      <c r="C933" t="s">
+        <v>1765</v>
+      </c>
+    </row>
+    <row r="934" spans="1:3">
+      <c r="A934">
+        <v>69</v>
+      </c>
+      <c r="B934" t="s">
+        <v>1766</v>
+      </c>
+      <c r="C934" t="s">
+        <v>1767</v>
+      </c>
+    </row>
+    <row r="935" spans="1:3">
+      <c r="A935">
+        <v>69</v>
+      </c>
+      <c r="B935" t="s">
+        <v>1768</v>
+      </c>
+      <c r="C935" t="s">
+        <v>1769</v>
+      </c>
+    </row>
+    <row r="936" spans="1:3">
+      <c r="A936">
+        <v>69</v>
+      </c>
+      <c r="B936" t="s">
+        <v>1770</v>
+      </c>
+      <c r="C936" t="s">
+        <v>1771</v>
+      </c>
+    </row>
+    <row r="937" spans="1:3">
+      <c r="A937">
+        <v>69</v>
+      </c>
+      <c r="B937" t="s">
+        <v>1772</v>
+      </c>
+      <c r="C937" t="s">
+        <v>1773</v>
+      </c>
+    </row>
+    <row r="938" spans="1:3">
+      <c r="A938">
+        <v>69</v>
+      </c>
+      <c r="B938" t="s">
+        <v>1774</v>
+      </c>
+      <c r="C938" t="s">
+        <v>1775</v>
+      </c>
+    </row>
+    <row r="939" spans="1:3">
+      <c r="A939">
+        <v>69</v>
+      </c>
+      <c r="B939" t="s">
+        <v>1776</v>
+      </c>
+      <c r="C939" t="s">
+        <v>1777</v>
+      </c>
+    </row>
+    <row r="940" spans="1:3">
+      <c r="A940">
+        <v>69</v>
+      </c>
+      <c r="B940" t="s">
+        <v>1778</v>
+      </c>
+      <c r="C940" t="s">
+        <v>1779</v>
+      </c>
+    </row>
+    <row r="941" spans="1:3">
+      <c r="A941">
+        <v>70</v>
+      </c>
+      <c r="B941" t="s">
+        <v>1780</v>
+      </c>
+      <c r="C941" t="s">
+        <v>1781</v>
+      </c>
+    </row>
+    <row r="942" spans="1:3">
+      <c r="A942">
+        <v>70</v>
+      </c>
+      <c r="B942" t="s">
+        <v>1656</v>
+      </c>
+      <c r="C942" t="s">
+        <v>1782</v>
+      </c>
+    </row>
+    <row r="943" spans="1:3">
+      <c r="A943">
+        <v>70</v>
+      </c>
+      <c r="B943" t="s">
+        <v>1783</v>
+      </c>
+      <c r="C943" t="s">
+        <v>1784</v>
+      </c>
+    </row>
+    <row r="944" spans="1:3">
+      <c r="A944">
+        <v>70</v>
+      </c>
+      <c r="B944" t="s">
+        <v>1786</v>
+      </c>
+      <c r="C944" t="s">
+        <v>1787</v>
+      </c>
+    </row>
+    <row r="945" spans="1:3">
+      <c r="A945">
+        <v>70</v>
+      </c>
+      <c r="B945" t="s">
+        <v>1788</v>
+      </c>
+      <c r="C945" t="s">
+        <v>1789</v>
+      </c>
+    </row>
+    <row r="946" spans="1:3">
+      <c r="A946">
+        <v>70</v>
+      </c>
+      <c r="B946" t="s">
+        <v>1790</v>
+      </c>
+      <c r="C946" t="s">
+        <v>1791</v>
+      </c>
+    </row>
+    <row r="947" spans="1:3">
+      <c r="A947">
+        <v>70</v>
+      </c>
+      <c r="B947" t="s">
+        <v>1792</v>
+      </c>
+      <c r="C947" t="s">
+        <v>1793</v>
+      </c>
+    </row>
+    <row r="948" spans="1:3">
+      <c r="A948">
+        <v>70</v>
+      </c>
+      <c r="B948" t="s">
+        <v>1794</v>
+      </c>
+      <c r="C948" t="s">
+        <v>1795</v>
+      </c>
+    </row>
+    <row r="949" spans="1:3">
+      <c r="A949">
+        <v>70</v>
+      </c>
+      <c r="B949" t="s">
+        <v>1796</v>
+      </c>
+      <c r="C949" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="950" spans="1:3">
+      <c r="A950">
+        <v>70</v>
+      </c>
+      <c r="B950" t="s">
+        <v>1797</v>
+      </c>
+      <c r="C950" t="s">
+        <v>1798</v>
+      </c>
+    </row>
+    <row r="951" spans="1:3">
+      <c r="A951">
+        <v>70</v>
+      </c>
+      <c r="B951" t="s">
+        <v>1799</v>
+      </c>
+      <c r="C951" t="s">
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="952" spans="1:3">
+      <c r="A952">
+        <v>70</v>
+      </c>
+      <c r="B952" t="s">
+        <v>1801</v>
+      </c>
+      <c r="C952" t="s">
+        <v>1802</v>
+      </c>
+    </row>
+    <row r="953" spans="1:3">
+      <c r="A953">
+        <v>70</v>
+      </c>
+      <c r="B953" t="s">
+        <v>1803</v>
+      </c>
+      <c r="C953" t="s">
+        <v>1804</v>
+      </c>
+    </row>
+    <row r="954" spans="1:3">
+      <c r="A954">
+        <v>70</v>
+      </c>
+      <c r="B954" t="s">
+        <v>1805</v>
+      </c>
+      <c r="C954" t="s">
+        <v>1806</v>
+      </c>
+    </row>
+    <row r="955" spans="1:3">
+      <c r="A955">
+        <v>70</v>
+      </c>
+      <c r="B955" t="s">
+        <v>1807</v>
+      </c>
+      <c r="C955" t="s">
+        <v>1806</v>
+      </c>
+    </row>
+    <row r="956" spans="1:3">
+      <c r="A956">
+        <v>70</v>
+      </c>
+      <c r="B956" t="s">
+        <v>1808</v>
+      </c>
+      <c r="C956" t="s">
+        <v>1806</v>
+      </c>
+    </row>
+    <row r="957" spans="1:3">
+      <c r="A957">
+        <v>70</v>
+      </c>
+      <c r="B957" t="s">
+        <v>1809</v>
+      </c>
+      <c r="C957" t="s">
+        <v>1810</v>
+      </c>
+    </row>
+    <row r="958" spans="1:3">
+      <c r="A958">
+        <v>70</v>
+      </c>
+      <c r="B958" t="s">
+        <v>1811</v>
+      </c>
+      <c r="C958" t="s">
+        <v>1812</v>
+      </c>
+    </row>
+    <row r="959" spans="1:3">
+      <c r="A959">
+        <v>70</v>
+      </c>
+      <c r="B959" t="s">
+        <v>1813</v>
+      </c>
+      <c r="C959" t="s">
+        <v>1814</v>
+      </c>
+    </row>
+    <row r="960" spans="1:3">
+      <c r="A960">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -14320,7 +17061,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
@@ -14336,6 +17079,9 @@
       </c>
       <c r="C1" s="3" t="s">
         <v>163</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1785</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="22" customHeight="1">

</xml_diff>